<commit_message>
fixed links, and updated to work with latest ecoinvent database
</commit_message>
<xml_diff>
--- a/excel_importer_example.xlsx
+++ b/excel_importer_example.xlsx
@@ -1,23 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maximilian Koslowski\bwSyncAndShare\PROSET (Simon Schulte)\5_Members\Max\Brightway\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deanhart/Documents/brightway2/notebooks/Brightway2_Intro/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103D992E-3EA3-3D44-B988-47503D8B6BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="0" windowWidth="28305" windowHeight="20520" activeTab="2"/>
+    <workbookView xWindow="22780" yWindow="-20820" windowWidth="28300" windowHeight="20480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="skip this sheet" sheetId="2" r:id="rId1"/>
     <sheet name="first process" sheetId="1" r:id="rId2"/>
     <sheet name="other process" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -26,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="61">
   <si>
     <t>Database</t>
   </si>
@@ -124,21 +135,12 @@
     <t>You can tell the importer to ignore some columns, where you can do calculations or take notes.</t>
   </si>
   <si>
-    <t xml:space="preserve">to start ignoring. Start counting columns from A (1), B (2), etc. </t>
-  </si>
-  <si>
-    <t>In this case, we will ignore columns J (10) and higher.</t>
-  </si>
-  <si>
     <t>cutoff</t>
   </si>
   <si>
     <t>You do this by putting the text `cutoff` in cell A1, and then the column number (it has to be a number) of the first column</t>
   </si>
   <si>
-    <t>There can be blank lines before the activity definitions.</t>
-  </si>
-  <si>
     <t>To skip sheets, cell A1 must be `skip`.</t>
   </si>
   <si>
@@ -215,12 +217,15 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>to start ignoring. Start counting columns from A (1), B (2), etc.  In this case, we will ignore columns J (10) and higher.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -272,6 +277,7 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -334,35 +340,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="29">
-    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -661,31 +667,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
@@ -701,27 +707,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="50.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B1">
         <v>10</v>
@@ -730,18 +736,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -749,154 +755,231 @@
         <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="C4" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="F13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14">
+        <v>0.33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11">
+      <c r="G14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0.33</v>
+      </c>
+      <c r="J14" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" t="s">
+        <v>23</v>
+      </c>
+      <c r="M14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15">
+        <v>0.33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0.33</v>
+      </c>
+      <c r="J15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C16" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16">
-        <v>0.33</v>
-      </c>
-      <c r="C16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" t="s">
-        <v>55</v>
+      <c r="D16" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F16" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="J16" t="s">
         <v>23</v>
@@ -911,12 +994,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>54</v>
       </c>
       <c r="B17">
-        <v>0.33</v>
+        <v>0.1</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -925,19 +1008,19 @@
         <v>55</v>
       </c>
       <c r="E17" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="G17" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
-      <c r="I17">
-        <v>0.33</v>
+      <c r="I17" t="s">
+        <v>23</v>
       </c>
       <c r="J17" t="s">
         <v>23</v>
@@ -949,88 +1032,6 @@
         <v>23</v>
       </c>
       <c r="M17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18" t="s">
-        <v>41</v>
-      </c>
-      <c r="G18" t="s">
-        <v>24</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-      <c r="J18" t="s">
-        <v>23</v>
-      </c>
-      <c r="K18" t="s">
-        <v>23</v>
-      </c>
-      <c r="L18" t="s">
-        <v>23</v>
-      </c>
-      <c r="M18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19">
-        <v>0.1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" t="s">
-        <v>58</v>
-      </c>
-      <c r="E19" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" t="s">
-        <v>23</v>
-      </c>
-      <c r="G19" t="s">
-        <v>60</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19" t="s">
-        <v>23</v>
-      </c>
-      <c r="J19" t="s">
-        <v>23</v>
-      </c>
-      <c r="K19" t="s">
-        <v>23</v>
-      </c>
-      <c r="L19" t="s">
-        <v>23</v>
-      </c>
-      <c r="M19" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1046,180 +1047,259 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B1">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P8">
+        <v>200</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O9" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B11">
+        <f>1/P8</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <f>B11</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11">
+        <f>I11/10</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="M11">
+        <f>I11*10</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="E12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>47</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="P10">
-        <v>200</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="P11">
-        <v>1</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13">
-        <f>1/P10</f>
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F13" t="s">
         <v>41</v>
       </c>
       <c r="G13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H13">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <f>B13</f>
-        <v>5.0000000000000001E-3</v>
+        <v>1</v>
       </c>
       <c r="J13" t="s">
         <v>23</v>
@@ -1227,94 +1307,10 @@
       <c r="K13" t="s">
         <v>23</v>
       </c>
-      <c r="L13">
-        <f>I13/10</f>
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="M13">
-        <f>I13*10</f>
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14" t="s">
-        <v>23</v>
-      </c>
-      <c r="K14" t="s">
-        <v>23</v>
-      </c>
-      <c r="L14" t="s">
-        <v>23</v>
-      </c>
-      <c r="M14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" t="s">
-        <v>24</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15" t="s">
-        <v>23</v>
-      </c>
-      <c r="K15" t="s">
-        <v>23</v>
-      </c>
-      <c r="L15" t="s">
-        <v>23</v>
-      </c>
-      <c r="M15" t="s">
+      <c r="L13" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed links, and updated to work with latest ecoinvent database (#1)
* fixed links, and updated to work with latest ecoinvent database
</commit_message>
<xml_diff>
--- a/excel_importer_example.xlsx
+++ b/excel_importer_example.xlsx
@@ -1,23 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maximilian Koslowski\bwSyncAndShare\PROSET (Simon Schulte)\5_Members\Max\Brightway\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deanhart/Documents/brightway2/notebooks/Brightway2_Intro/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103D992E-3EA3-3D44-B988-47503D8B6BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="0" windowWidth="28305" windowHeight="20520" activeTab="2"/>
+    <workbookView xWindow="22780" yWindow="-20820" windowWidth="28300" windowHeight="20480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="skip this sheet" sheetId="2" r:id="rId1"/>
     <sheet name="first process" sheetId="1" r:id="rId2"/>
     <sheet name="other process" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -26,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="61">
   <si>
     <t>Database</t>
   </si>
@@ -124,21 +135,12 @@
     <t>You can tell the importer to ignore some columns, where you can do calculations or take notes.</t>
   </si>
   <si>
-    <t xml:space="preserve">to start ignoring. Start counting columns from A (1), B (2), etc. </t>
-  </si>
-  <si>
-    <t>In this case, we will ignore columns J (10) and higher.</t>
-  </si>
-  <si>
     <t>cutoff</t>
   </si>
   <si>
     <t>You do this by putting the text `cutoff` in cell A1, and then the column number (it has to be a number) of the first column</t>
   </si>
   <si>
-    <t>There can be blank lines before the activity definitions.</t>
-  </si>
-  <si>
     <t>To skip sheets, cell A1 must be `skip`.</t>
   </si>
   <si>
@@ -215,12 +217,15 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>to start ignoring. Start counting columns from A (1), B (2), etc.  In this case, we will ignore columns J (10) and higher.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -272,6 +277,7 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -334,35 +340,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="29">
-    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -661,31 +667,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
@@ -701,27 +707,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="50.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B1">
         <v>10</v>
@@ -730,18 +736,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -749,154 +755,231 @@
         <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="C4" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="F13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14">
+        <v>0.33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11">
+      <c r="G14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0.33</v>
+      </c>
+      <c r="J14" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" t="s">
+        <v>23</v>
+      </c>
+      <c r="M14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15">
+        <v>0.33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0.33</v>
+      </c>
+      <c r="J15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C16" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16">
-        <v>0.33</v>
-      </c>
-      <c r="C16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" t="s">
-        <v>55</v>
+      <c r="D16" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F16" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="J16" t="s">
         <v>23</v>
@@ -911,12 +994,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>54</v>
       </c>
       <c r="B17">
-        <v>0.33</v>
+        <v>0.1</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -925,19 +1008,19 @@
         <v>55</v>
       </c>
       <c r="E17" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="G17" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
-      <c r="I17">
-        <v>0.33</v>
+      <c r="I17" t="s">
+        <v>23</v>
       </c>
       <c r="J17" t="s">
         <v>23</v>
@@ -949,88 +1032,6 @@
         <v>23</v>
       </c>
       <c r="M17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18" t="s">
-        <v>41</v>
-      </c>
-      <c r="G18" t="s">
-        <v>24</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-      <c r="J18" t="s">
-        <v>23</v>
-      </c>
-      <c r="K18" t="s">
-        <v>23</v>
-      </c>
-      <c r="L18" t="s">
-        <v>23</v>
-      </c>
-      <c r="M18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19">
-        <v>0.1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" t="s">
-        <v>58</v>
-      </c>
-      <c r="E19" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" t="s">
-        <v>23</v>
-      </c>
-      <c r="G19" t="s">
-        <v>60</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19" t="s">
-        <v>23</v>
-      </c>
-      <c r="J19" t="s">
-        <v>23</v>
-      </c>
-      <c r="K19" t="s">
-        <v>23</v>
-      </c>
-      <c r="L19" t="s">
-        <v>23</v>
-      </c>
-      <c r="M19" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1046,180 +1047,259 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B1">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P8">
+        <v>200</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O9" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B11">
+        <f>1/P8</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <f>B11</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11">
+        <f>I11/10</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="M11">
+        <f>I11*10</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="E12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>47</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="P10">
-        <v>200</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="P11">
-        <v>1</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13">
-        <f>1/P10</f>
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F13" t="s">
         <v>41</v>
       </c>
       <c r="G13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H13">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <f>B13</f>
-        <v>5.0000000000000001E-3</v>
+        <v>1</v>
       </c>
       <c r="J13" t="s">
         <v>23</v>
@@ -1227,94 +1307,10 @@
       <c r="K13" t="s">
         <v>23</v>
       </c>
-      <c r="L13">
-        <f>I13/10</f>
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="M13">
-        <f>I13*10</f>
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14" t="s">
-        <v>23</v>
-      </c>
-      <c r="K14" t="s">
-        <v>23</v>
-      </c>
-      <c r="L14" t="s">
-        <v>23</v>
-      </c>
-      <c r="M14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" t="s">
-        <v>24</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15" t="s">
-        <v>23</v>
-      </c>
-      <c r="K15" t="s">
-        <v>23</v>
-      </c>
-      <c r="L15" t="s">
-        <v>23</v>
-      </c>
-      <c r="M15" t="s">
+      <c r="L13" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>